<commit_message>
add new test code
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -375,22 +375,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -430,7 +430,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -440,7 +440,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -450,12 +450,12 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">

</xml_diff>

<commit_message>
refactored medianBlur.py and benchmarking.py
</commit_message>
<xml_diff>
--- a/testfile.xlsx
+++ b/testfile.xlsx
@@ -380,27 +380,27 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>48</v>
+        <v>937</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>89</v>
+        <v>20536</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>12</v>
+        <v>8437</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -420,47 +420,47 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
@@ -495,12 +495,12 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">

</xml_diff>